<commit_message>
Update Element dataset and created ensemble net
</commit_message>
<xml_diff>
--- a/Packages/ThermoClassifier/ThermoClassifier/phases/models/Model statistics.xlsx
+++ b/Packages/ThermoClassifier/ThermoClassifier/phases/models/Model statistics.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\Documents\Montanuni\Masterarbeit\5_Programmcodes\Neural_Nets\Classification\PhaseClassifier\Models\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\Documents\Montanuni\Masterarbeit\5 Programmcodes\packages\thermoclassifier\thermoclassifier\phases\models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA084264-56D8-4B38-83D1-A59986265C81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C25C3E2B-CD49-4E28-A4F9-4A0D5FE697AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2547,7 +2547,7 @@
   <dimension ref="A1:E77"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>